<commit_message>
completed test_login/need add case
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -71,10 +71,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -84,23 +84,23 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -127,9 +127,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -140,39 +156,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -194,6 +187,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -210,7 +211,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,15 +219,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,13 +249,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,169 +429,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,6 +440,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -454,24 +463,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,6 +484,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -502,11 +504,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -546,38 +546,38 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -586,101 +586,101 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -691,6 +691,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" quotePrefix="1">
@@ -1018,7 +1021,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -1061,7 +1064,7 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2"/>
@@ -1074,10 +1077,10 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1104,10 +1107,10 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1119,7 +1122,7 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1134,14 +1137,14 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="3"/>
@@ -1203,6 +1206,9 @@
       <c r="G14" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D8" r:id="rId1" display="https://tomorning.me:20001/m/layoutmgt/showall" tooltip="https://tomorning.me:20001/m/layoutmgt/showall"/>
+  </hyperlinks>
   <pageMargins left="0.697916666666667" right="0.697916666666667" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>

</xml_diff>